<commit_message>
issues & new jobs
</commit_message>
<xml_diff>
--- a/Jobs to do.xlsx
+++ b/Jobs to do.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>questionnaire confirmation page</t>
+  </si>
+  <si>
+    <t>Validation</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="1">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -735,6 +738,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
       <c r="D16" t="s">
         <v>29</v>
       </c>
@@ -743,6 +749,14 @@
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>